<commit_message>
updated point source run average
</commit_message>
<xml_diff>
--- a/PLOT_TEMPLATE.xlsx
+++ b/PLOT_TEMPLATE.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\210Pb_thismachine\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9985E541-558B-427A-AD7D-48C4B1FF850E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="405" yWindow="765" windowWidth="25440" windowHeight="14415" tabRatio="711" activeTab="1"/>
+    <workbookView xWindow="34530" yWindow="0" windowWidth="23325" windowHeight="15585" tabRatio="711" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Core Details" sheetId="7" r:id="rId1"/>
@@ -14,8 +20,8 @@
     <sheet name="Excess Pb-210" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029" refMode="R1C1"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -376,13 +382,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -540,7 +546,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -693,6 +699,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -712,9 +719,18 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:style val="1"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -742,7 +758,7 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -750,11 +766,33 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -911,14 +949,20 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:smooth val="0"/>
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000001F-B61B-4602-9470-03A2FF4DDD45}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:axId val="78924800"/>
         <c:axId val="79438976"/>
@@ -930,6 +974,7 @@
           <c:max val="100"/>
           <c:min val="0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="t"/>
         <c:majorGridlines>
           <c:spPr>
@@ -947,6 +992,7 @@
         </c:majorGridlines>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -991,6 +1037,7 @@
           <c:orientation val="maxMin"/>
           <c:max val="35"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1008,6 +1055,7 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1056,6 +1104,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1091,9 +1140,18 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:style val="1"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1118,6 +1176,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
           <a:srgbClr val="FFFF00"/>
@@ -1128,6 +1187,7 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -1142,6 +1202,7 @@
       </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1204,6 +1265,7 @@
             <c:errDir val="x"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'Excess Pb-210'!$I$3:$I$8</c:f>
@@ -1275,6 +1337,7 @@
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
+            <c:noEndCap val="0"/>
             <c:val val="1"/>
             <c:spPr>
               <a:noFill/>
@@ -1408,7 +1471,8 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:smooth val="0"/>
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3899-487D-A472-ACF84E9C1B1E}"/>
             </c:ext>
@@ -1476,6 +1540,7 @@
             <c:errDir val="x"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'Excess Pb-210'!$Q$3:$Q$8</c:f>
@@ -1547,6 +1612,7 @@
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
+            <c:noEndCap val="0"/>
             <c:val val="1"/>
             <c:spPr>
               <a:noFill/>
@@ -1680,7 +1746,8 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:smooth val="0"/>
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-3899-487D-A472-ACF84E9C1B1E}"/>
             </c:ext>
@@ -1748,6 +1815,7 @@
             <c:errDir val="x"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'Excess Pb-210'!$T$3:$T$8</c:f>
@@ -1819,6 +1887,7 @@
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
+            <c:noEndCap val="0"/>
             <c:val val="1"/>
             <c:spPr>
               <a:noFill/>
@@ -1952,13 +2021,21 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:smooth val="0"/>
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-3899-487D-A472-ACF84E9C1B1E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:axId val="81597184"/>
         <c:axId val="81598720"/>
       </c:scatterChart>
@@ -1968,6 +2045,7 @@
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="t"/>
         <c:majorGridlines>
           <c:spPr>
@@ -2006,6 +2084,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -2016,6 +2095,7 @@
         </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2056,6 +2136,7 @@
           <c:orientation val="maxMin"/>
           <c:min val="0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -2094,6 +2175,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -2104,6 +2186,7 @@
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2158,6 +2241,7 @@
           <c:h val="0.14422765282727551"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2185,7 +2269,8 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
@@ -2227,9 +2312,18 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:style val="1"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2270,14 +2364,7 @@
           </a:p>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1680" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx2"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
+              <a:defRPr/>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
@@ -2294,6 +2381,7 @@
           <c:y val="3.6117195410491389E-2"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
           <a:srgbClr val="FFFF00"/>
@@ -2303,7 +2391,25 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1680" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -2318,6 +2424,7 @@
       </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -2386,6 +2493,7 @@
             <c:errDir val="x"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'Excess Pb-210'!$V$3:$V$19</c:f>
@@ -2523,6 +2631,7 @@
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
+            <c:noEndCap val="0"/>
             <c:val val="0"/>
             <c:spPr>
               <a:noFill/>
@@ -2657,7 +2766,8 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:smooth val="0"/>
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-9678-4E18-AF5C-BB7950C10E2F}"/>
             </c:ext>
@@ -2732,7 +2842,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{48F00EA2-0FE1-D74A-B96D-F33E8934E444}" type="CELLRANGE">
+                    <a:fld id="{53160187-E378-479E-8CE0-7334B3A61826}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2742,7 +2852,13 @@
                 </c:rich>
               </c:tx>
               <c:dLblPos val="r"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
@@ -2760,7 +2876,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DC2EDAC5-A530-FB49-B1AB-F6E30D1F0AB5}" type="CELLRANGE">
+                    <a:fld id="{4F7E36C1-5FD7-40D6-B736-ABBD3E3C2CA5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2770,7 +2886,13 @@
                 </c:rich>
               </c:tx>
               <c:dLblPos val="r"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
@@ -2788,7 +2910,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DDCF0AE9-D996-4344-A966-299153BFFA33}" type="CELLRANGE">
+                    <a:fld id="{92388FF8-A1BA-4FDA-9BCE-E3E45464ED69}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2798,7 +2920,13 @@
                 </c:rich>
               </c:tx>
               <c:dLblPos val="r"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
@@ -2816,7 +2944,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F1974421-C582-094F-9968-1F1EB45A4754}" type="CELLRANGE">
+                    <a:fld id="{6B2EE2CD-1E2B-42FB-A424-9FE2ACF006C8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2826,7 +2954,13 @@
                 </c:rich>
               </c:tx>
               <c:dLblPos val="r"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
@@ -2844,7 +2978,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{91AA01A9-E6CC-8545-9D26-43E5BA00A23A}" type="CELLRANGE">
+                    <a:fld id="{980BA693-80E8-492D-BBE4-F90836EA17AE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2854,7 +2988,13 @@
                 </c:rich>
               </c:tx>
               <c:dLblPos val="r"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
@@ -2872,7 +3012,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{51E13A79-8204-8047-99F1-14FCB91F858B}" type="CELLRANGE">
+                    <a:fld id="{37F58830-D236-4B48-98EA-0107D879B5A1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2882,7 +3022,13 @@
                 </c:rich>
               </c:tx>
               <c:dLblPos val="r"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
@@ -2900,7 +3046,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{83DA516D-7443-344D-BE2F-1B3446F6150A}" type="CELLRANGE">
+                    <a:fld id="{BF4E1BB8-2A37-44B9-BA8B-BC36BD148E50}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2910,7 +3056,13 @@
                 </c:rich>
               </c:tx>
               <c:dLblPos val="r"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
@@ -2928,7 +3080,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{542E74EA-CF56-E143-9485-631F006F4967}" type="CELLRANGE">
+                    <a:fld id="{646F8607-2AB2-4C92-8F1E-62C79C222B17}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2938,7 +3090,13 @@
                 </c:rich>
               </c:tx>
               <c:dLblPos val="r"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
@@ -2956,7 +3114,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{311FB030-438D-A44A-8963-EF639DB42BCE}" type="CELLRANGE">
+                    <a:fld id="{BC4F89E3-C8E2-40DC-ABB1-C7852586EB29}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2966,7 +3124,13 @@
                 </c:rich>
               </c:tx>
               <c:dLblPos val="r"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
@@ -2984,7 +3148,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{319D29CD-AAE8-CD4A-A46B-9497C06D8666}" type="CELLRANGE">
+                    <a:fld id="{48EB8BCB-136B-4B12-99BF-337B293AB062}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2994,7 +3158,13 @@
                 </c:rich>
               </c:tx>
               <c:dLblPos val="r"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
@@ -3012,7 +3182,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DAA59E85-3217-F44C-BD60-4B0075557EDC}" type="CELLRANGE">
+                    <a:fld id="{CB56EF0F-2B65-479A-B0C2-06EBBD825059}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3022,7 +3192,13 @@
                 </c:rich>
               </c:tx>
               <c:dLblPos val="r"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
@@ -3040,7 +3216,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4E0DA257-8BB2-6547-9ACE-12CF77835BAC}" type="CELLRANGE">
+                    <a:fld id="{C18F38AA-D060-4155-9C43-474FB84E62E1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3050,7 +3226,13 @@
                 </c:rich>
               </c:tx>
               <c:dLblPos val="r"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
@@ -3068,7 +3250,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{86FE19FE-3094-B64B-9846-016CF1613168}" type="CELLRANGE">
+                    <a:fld id="{9B83BFB2-226D-4888-9225-134B63E9E568}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3078,7 +3260,13 @@
                 </c:rich>
               </c:tx>
               <c:dLblPos val="r"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
@@ -3096,7 +3284,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{17C9B1A0-BC9E-FF44-8DE9-194A87F23CF9}" type="CELLRANGE">
+                    <a:fld id="{C9D7F62F-2176-4EBF-9730-55D79F3D4A78}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3106,7 +3294,13 @@
                 </c:rich>
               </c:tx>
               <c:dLblPos val="r"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
@@ -3124,7 +3318,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{53F64B40-B9DD-ED41-8575-CB36812E2646}" type="CELLRANGE">
+                    <a:fld id="{36F95C01-7535-4A36-9398-52B1BC90D4D2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3134,7 +3328,13 @@
                 </c:rich>
               </c:tx>
               <c:dLblPos val="r"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
@@ -3152,7 +3352,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C239E253-73DD-6D40-806B-CB643EB9E47B}" type="CELLRANGE">
+                    <a:fld id="{EFCA44A8-0B8A-41FF-8F96-DB38826157B6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3162,7 +3362,13 @@
                 </c:rich>
               </c:tx>
               <c:dLblPos val="r"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
@@ -3180,7 +3386,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2068FA62-C97D-DA40-9E7C-3E672154A3F8}" type="CELLRANGE">
+                    <a:fld id="{9B2A5953-3FCF-44E4-856B-3043E9B0ED66}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3190,7 +3396,13 @@
                 </c:rich>
               </c:tx>
               <c:dLblPos val="r"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
@@ -3201,7 +3413,6 @@
                 </c:ext>
               </c:extLst>
             </c:dLbl>
-            <c:delete val="1"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -3229,7 +3440,14 @@
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showDataLabelsRange val="1"/>
                 <c15:showLeaderLines val="1"/>
@@ -3253,6 +3471,7 @@
             <c:errDir val="x"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'Excess Pb-210'!$J$3:$J$19</c:f>
@@ -3390,6 +3609,7 @@
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
+            <c:noEndCap val="0"/>
             <c:val val="0"/>
             <c:spPr>
               <a:noFill/>
@@ -3524,7 +3744,8 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:smooth val="0"/>
+          <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
                 <c15:f>'Excess Pb-210'!$AA$3:$AA$19</c15:f>
@@ -3590,7 +3811,12 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:axId val="83801216"/>
         <c:axId val="83802752"/>
@@ -3601,6 +3827,7 @@
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="t"/>
         <c:majorGridlines>
           <c:spPr>
@@ -3618,6 +3845,7 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -3658,6 +3886,7 @@
           <c:orientation val="maxMin"/>
           <c:min val="0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -3696,6 +3925,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -3703,9 +3933,27 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -3761,6 +4009,7 @@
           <c:h val="7.8795125981642317E-2"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -3788,7 +4037,8 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
@@ -3857,33 +4107,6 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
-  <a:schemeClr val="dk1"/>
-  <cs:variation>
-    <a:tint val="88500"/>
-  </cs:variation>
-  <cs:variation>
-    <a:tint val="55000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:tint val="75000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:tint val="98500"/>
-  </cs:variation>
-  <cs:variation>
-    <a:tint val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:tint val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:tint val="80000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
   <a:schemeClr val="dk1"/>
   <cs:variation>
@@ -4905,485 +5128,6 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="242">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk2">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="2"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="2"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="2"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="2"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="2"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="60000"/>
-            <a:lumOff val="40000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="60000"/>
-            <a:lumOff val="40000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="60000"/>
-            <a:lumOff val="40000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="40000"/>
-            <a:lumOff val="60000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -5404,7 +5148,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5445,7 +5189,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FC0388C9-30A4-4A20-A0F9-F89E746B6912}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC0388C9-30A4-4A20-A0F9-F89E746B6912}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5481,7 +5225,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DF88E717-4BB8-4472-9410-C6EE152E7DD9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF88E717-4BB8-4472-9410-C6EE152E7DD9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5793,14 +5537,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N21"/>
   <sheetViews>
@@ -5808,7 +5552,7 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.42578125" style="7" customWidth="1"/>
     <col min="2" max="2" width="56.7109375" style="8" customWidth="1"/>
@@ -5824,7 +5568,7 @@
     <col min="15" max="16384" width="8.85546875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="9" customFormat="1" ht="15">
+    <row r="1" spans="1:14" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>28</v>
       </c>
@@ -5844,7 +5588,7 @@
       <c r="M1" s="10"/>
       <c r="N1" s="10"/>
     </row>
-    <row r="2" spans="1:14" ht="15">
+    <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>27</v>
       </c>
@@ -5852,7 +5596,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15">
+    <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>33</v>
       </c>
@@ -5860,7 +5604,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15">
+    <row r="4" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>32</v>
       </c>
@@ -5868,7 +5612,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15">
+    <row r="5" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>34</v>
       </c>
@@ -5876,7 +5620,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15">
+    <row r="6" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>47</v>
       </c>
@@ -5884,7 +5628,7 @@
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:14" ht="15">
+    <row r="7" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>35</v>
       </c>
@@ -5894,7 +5638,7 @@
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:14" ht="15">
+    <row r="8" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>61</v>
       </c>
@@ -5902,7 +5646,7 @@
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:14" ht="15">
+    <row r="9" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>62</v>
       </c>
@@ -5910,7 +5654,7 @@
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:14" ht="15">
+    <row r="10" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>46</v>
       </c>
@@ -5918,7 +5662,7 @@
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:14" ht="15">
+    <row r="11" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>31</v>
       </c>
@@ -5926,7 +5670,7 @@
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:14" ht="15">
+    <row r="12" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>48</v>
       </c>
@@ -5934,7 +5678,7 @@
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:14" ht="30">
+    <row r="13" spans="1:14" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
         <v>49</v>
       </c>
@@ -5942,7 +5686,7 @@
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:14" ht="45">
+    <row r="14" spans="1:14" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
         <v>50</v>
       </c>
@@ -5950,7 +5694,7 @@
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:14" ht="15">
+    <row r="15" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
         <v>51</v>
       </c>
@@ -5958,7 +5702,7 @@
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:14" ht="15">
+    <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>30</v>
       </c>
@@ -5966,7 +5710,7 @@
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" ht="14.1" customHeight="1">
+    <row r="17" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="55" t="s">
         <v>29</v>
       </c>
@@ -5974,17 +5718,17 @@
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="55"/>
       <c r="B18" s="57"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>59</v>
       </c>
@@ -6000,14 +5744,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="V26" sqref="V26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="14.140625" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
@@ -6016,7 +5760,7 @@
     <col min="13" max="13" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E1" s="58" t="s">
         <v>55</v>
       </c>
@@ -6029,7 +5773,7 @@
       </c>
       <c r="K1" s="58"/>
     </row>
-    <row r="2" spans="1:14" ht="60.75" customHeight="1">
+    <row r="2" spans="1:14" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -6073,7 +5817,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>'Core Details'!B7</f>
         <v>XXXX</v>
@@ -6120,7 +5864,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>A3</f>
         <v>XXXX</v>
@@ -6167,7 +5911,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f t="shared" ref="A5:A19" si="5">A4</f>
         <v>XXXX</v>
@@ -6214,7 +5958,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f t="shared" si="5"/>
         <v>XXXX</v>
@@ -6261,7 +6005,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f t="shared" si="5"/>
         <v>XXXX</v>
@@ -6308,7 +6052,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f t="shared" si="5"/>
         <v>XXXX</v>
@@ -6355,7 +6099,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f t="shared" si="5"/>
         <v>XXXX</v>
@@ -6402,7 +6146,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f t="shared" si="5"/>
         <v>XXXX</v>
@@ -6449,7 +6193,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f t="shared" si="5"/>
         <v>XXXX</v>
@@ -6496,7 +6240,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" si="5"/>
         <v>XXXX</v>
@@ -6543,7 +6287,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f t="shared" si="5"/>
         <v>XXXX</v>
@@ -6590,7 +6334,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f t="shared" si="5"/>
         <v>XXXX</v>
@@ -6637,7 +6381,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f t="shared" si="5"/>
         <v>XXXX</v>
@@ -6684,7 +6428,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f t="shared" si="5"/>
         <v>XXXX</v>
@@ -6731,7 +6475,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f t="shared" si="5"/>
         <v>XXXX</v>
@@ -6778,7 +6522,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f t="shared" si="5"/>
         <v>XXXX</v>
@@ -6825,7 +6569,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f t="shared" si="5"/>
         <v>XXXX</v>
@@ -6885,21 +6629,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="16" customFormat="1" ht="75">
+    <row r="1" spans="1:9" s="16" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>36</v>
       </c>
@@ -6919,7 +6666,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.45" customHeight="1">
+    <row r="2" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="59" t="s">
         <v>42</v>
       </c>
@@ -6929,20 +6676,18 @@
       <c r="C2" s="14">
         <v>43965</v>
       </c>
-      <c r="D2">
-        <f>1.510473*100000</f>
-        <v>151047.29999999999</v>
-      </c>
-      <c r="E2">
-        <f>5.559227*10^3</f>
-        <v>5559.2269999999999</v>
-      </c>
-      <c r="G2" s="21">
+      <c r="D2" s="17">
+        <v>128883</v>
+      </c>
+      <c r="E2" s="17">
+        <v>4743.82</v>
+      </c>
+      <c r="G2" s="62">
         <f>AVERAGE(D2:D11)</f>
-        <v>151031.56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>128902.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="59"/>
       <c r="B3">
         <v>2</v>
@@ -6950,16 +6695,14 @@
       <c r="C3" s="14">
         <v>43965</v>
       </c>
-      <c r="D3">
-        <f>1.50964*100000</f>
-        <v>150964</v>
-      </c>
-      <c r="E3">
-        <f>5.55618*10^3</f>
-        <v>5556.18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="D3" s="17">
+        <v>128782</v>
+      </c>
+      <c r="E3" s="17">
+        <v>4740.12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="59"/>
       <c r="B4">
         <v>3</v>
@@ -6967,16 +6710,14 @@
       <c r="C4" s="14">
         <v>43965</v>
       </c>
-      <c r="D4">
-        <f>1.508569*100000</f>
-        <v>150856.9</v>
-      </c>
-      <c r="E4">
-        <f>5.55222*1000</f>
-        <v>5552.22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="D4" s="17">
+        <v>128879</v>
+      </c>
+      <c r="E4" s="17">
+        <v>4743.68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="59"/>
       <c r="B5">
         <v>4</v>
@@ -6984,17 +6725,15 @@
       <c r="C5" s="14">
         <v>43965</v>
       </c>
-      <c r="D5">
-        <f>1.50879*100000</f>
-        <v>150879</v>
-      </c>
-      <c r="E5">
-        <f>5.55302*1000</f>
-        <v>5553.02</v>
+      <c r="D5" s="17">
+        <v>129238</v>
+      </c>
+      <c r="E5" s="17">
+        <v>4756.8900000000003</v>
       </c>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="59"/>
       <c r="B6">
         <v>5</v>
@@ -7002,16 +6741,14 @@
       <c r="C6" s="14">
         <v>43965</v>
       </c>
-      <c r="D6">
-        <f>1.510106*100000</f>
-        <v>151010.6</v>
-      </c>
-      <c r="E6">
-        <f>5.557874*1000</f>
-        <v>5557.8739999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="D6" s="17">
+        <v>128671</v>
+      </c>
+      <c r="E6" s="17">
+        <v>4736.04</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="59"/>
       <c r="B7">
         <v>6</v>
@@ -7019,16 +6756,14 @@
       <c r="C7" s="14">
         <v>43965</v>
       </c>
-      <c r="D7">
-        <f>1.510267*100000</f>
-        <v>151026.70000000001</v>
-      </c>
-      <c r="E7">
-        <f>5.558465*1000</f>
-        <v>5558.4650000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="D7" s="17">
+        <v>128922</v>
+      </c>
+      <c r="E7" s="17">
+        <v>4745.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="59"/>
       <c r="B8">
         <v>7</v>
@@ -7036,16 +6771,14 @@
       <c r="C8" s="14">
         <v>43965</v>
       </c>
-      <c r="D8">
-        <f>1.512138*100000</f>
-        <v>151213.79999999999</v>
-      </c>
-      <c r="E8">
-        <f>5.565349*1000</f>
-        <v>5565.3490000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="D8" s="17">
+        <v>129029</v>
+      </c>
+      <c r="E8" s="17">
+        <v>4749.1899999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="59"/>
       <c r="B9">
         <v>8</v>
@@ -7053,16 +6786,14 @@
       <c r="C9" s="14">
         <v>43966</v>
       </c>
-      <c r="D9">
-        <f>1.510564*100000</f>
-        <v>151056.4</v>
-      </c>
-      <c r="E9">
-        <f>5.559558*1000</f>
-        <v>5559.558</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="D9" s="17">
+        <v>128887</v>
+      </c>
+      <c r="E9" s="17">
+        <v>4743.95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="59"/>
       <c r="B10">
         <v>9</v>
@@ -7070,16 +6801,14 @@
       <c r="C10" s="14">
         <v>43966</v>
       </c>
-      <c r="D10">
-        <f>1.509937*100000</f>
-        <v>150993.70000000001</v>
-      </c>
-      <c r="E10">
-        <f>5.557252*1000</f>
-        <v>5557.2520000000004</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="D10" s="17">
+        <v>128787</v>
+      </c>
+      <c r="E10" s="17">
+        <v>4740.3100000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="59"/>
       <c r="B11">
         <v>10</v>
@@ -7087,31 +6816,29 @@
       <c r="C11" s="14">
         <v>43966</v>
       </c>
-      <c r="D11">
-        <f>1.512672*100000</f>
-        <v>151267.20000000001</v>
-      </c>
-      <c r="E11">
-        <f>5.567313*1000</f>
-        <v>5567.3130000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="33.75">
+      <c r="D11" s="17">
+        <v>128947</v>
+      </c>
+      <c r="E11" s="17">
+        <v>4746.17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="33.75" x14ac:dyDescent="0.5">
       <c r="E13" t="s">
         <v>43</v>
       </c>
       <c r="I13" s="26"/>
     </row>
-    <row r="14" spans="1:9">
-      <c r="E14">
-        <f>AVERAGE(E2:E6)</f>
-        <v>5555.7042000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="3:3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E14" s="17">
+        <f>AVERAGE(E2:E11)</f>
+        <v>4744.5419999999995</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C22" s="14"/>
     </row>
-    <row r="23" spans="3:3">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C23" s="14"/>
     </row>
   </sheetData>
@@ -7124,7 +6851,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:N32"/>
   <sheetViews>
@@ -7132,7 +6859,7 @@
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9.140625" style="17"/>
     <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -7141,7 +6868,7 @@
     <col min="12" max="12" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -7151,7 +6878,7 @@
       <c r="H1" s="60"/>
       <c r="I1" s="60"/>
     </row>
-    <row r="2" spans="1:14" s="24" customFormat="1" ht="90">
+    <row r="2" spans="1:14" s="24" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
@@ -7188,7 +6915,7 @@
       <c r="M2" s="16"/>
       <c r="N2" s="16"/>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="str">
         <f>'Core Details'!B2</f>
         <v>XXXX (Ex: NBP2002)</v>
@@ -7213,7 +6940,7 @@
       </c>
       <c r="G3">
         <f>'Point source runs'!G2</f>
-        <v>151031.56</v>
+        <v>128902.5</v>
       </c>
       <c r="H3" s="49" t="s">
         <v>95</v>
@@ -7231,7 +6958,7 @@
       </c>
       <c r="M3" s="21"/>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="str">
         <f>A3</f>
         <v>XXXX (Ex: NBP2002)</v>
@@ -7256,7 +6983,7 @@
       </c>
       <c r="G4">
         <f>G3</f>
-        <v>151031.56</v>
+        <v>128902.5</v>
       </c>
       <c r="H4" s="49" t="s">
         <v>95</v>
@@ -7273,7 +7000,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="str">
         <f t="shared" ref="A5:A19" si="2">A4</f>
         <v>XXXX (Ex: NBP2002)</v>
@@ -7298,7 +7025,7 @@
       </c>
       <c r="G5">
         <f t="shared" ref="G5:G19" si="3">G4</f>
-        <v>151031.56</v>
+        <v>128902.5</v>
       </c>
       <c r="H5" s="49" t="s">
         <v>95</v>
@@ -7315,7 +7042,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="str">
         <f t="shared" si="2"/>
         <v>XXXX (Ex: NBP2002)</v>
@@ -7340,7 +7067,7 @@
       </c>
       <c r="G6">
         <f t="shared" si="3"/>
-        <v>151031.56</v>
+        <v>128902.5</v>
       </c>
       <c r="H6" s="49" t="s">
         <v>95</v>
@@ -7357,7 +7084,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="str">
         <f t="shared" si="2"/>
         <v>XXXX (Ex: NBP2002)</v>
@@ -7382,7 +7109,7 @@
       </c>
       <c r="G7">
         <f t="shared" si="3"/>
-        <v>151031.56</v>
+        <v>128902.5</v>
       </c>
       <c r="H7" s="49" t="s">
         <v>95</v>
@@ -7399,7 +7126,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="str">
         <f t="shared" si="2"/>
         <v>XXXX (Ex: NBP2002)</v>
@@ -7424,7 +7151,7 @@
       </c>
       <c r="G8">
         <f t="shared" si="3"/>
-        <v>151031.56</v>
+        <v>128902.5</v>
       </c>
       <c r="H8" s="49" t="s">
         <v>95</v>
@@ -7441,7 +7168,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="str">
         <f t="shared" si="2"/>
         <v>XXXX (Ex: NBP2002)</v>
@@ -7466,7 +7193,7 @@
       </c>
       <c r="G9">
         <f t="shared" si="3"/>
-        <v>151031.56</v>
+        <v>128902.5</v>
       </c>
       <c r="H9" s="49" t="s">
         <v>95</v>
@@ -7483,7 +7210,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="str">
         <f t="shared" si="2"/>
         <v>XXXX (Ex: NBP2002)</v>
@@ -7508,7 +7235,7 @@
       </c>
       <c r="G10">
         <f t="shared" si="3"/>
-        <v>151031.56</v>
+        <v>128902.5</v>
       </c>
       <c r="H10" s="49" t="s">
         <v>95</v>
@@ -7525,7 +7252,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="str">
         <f t="shared" si="2"/>
         <v>XXXX (Ex: NBP2002)</v>
@@ -7550,7 +7277,7 @@
       </c>
       <c r="G11">
         <f t="shared" si="3"/>
-        <v>151031.56</v>
+        <v>128902.5</v>
       </c>
       <c r="H11" s="49" t="s">
         <v>95</v>
@@ -7567,7 +7294,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="str">
         <f t="shared" si="2"/>
         <v>XXXX (Ex: NBP2002)</v>
@@ -7592,7 +7319,7 @@
       </c>
       <c r="G12">
         <f t="shared" si="3"/>
-        <v>151031.56</v>
+        <v>128902.5</v>
       </c>
       <c r="H12" s="49" t="s">
         <v>95</v>
@@ -7609,7 +7336,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="str">
         <f t="shared" si="2"/>
         <v>XXXX (Ex: NBP2002)</v>
@@ -7634,7 +7361,7 @@
       </c>
       <c r="G13">
         <f t="shared" si="3"/>
-        <v>151031.56</v>
+        <v>128902.5</v>
       </c>
       <c r="H13" s="49" t="s">
         <v>95</v>
@@ -7651,7 +7378,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="str">
         <f t="shared" si="2"/>
         <v>XXXX (Ex: NBP2002)</v>
@@ -7676,7 +7403,7 @@
       </c>
       <c r="G14">
         <f t="shared" si="3"/>
-        <v>151031.56</v>
+        <v>128902.5</v>
       </c>
       <c r="H14" s="49" t="s">
         <v>95</v>
@@ -7693,7 +7420,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="str">
         <f t="shared" si="2"/>
         <v>XXXX (Ex: NBP2002)</v>
@@ -7718,7 +7445,7 @@
       </c>
       <c r="G15">
         <f t="shared" si="3"/>
-        <v>151031.56</v>
+        <v>128902.5</v>
       </c>
       <c r="H15" s="49" t="s">
         <v>95</v>
@@ -7735,7 +7462,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="str">
         <f t="shared" si="2"/>
         <v>XXXX (Ex: NBP2002)</v>
@@ -7760,7 +7487,7 @@
       </c>
       <c r="G16">
         <f t="shared" si="3"/>
-        <v>151031.56</v>
+        <v>128902.5</v>
       </c>
       <c r="H16" s="49" t="s">
         <v>95</v>
@@ -7777,7 +7504,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="str">
         <f t="shared" si="2"/>
         <v>XXXX (Ex: NBP2002)</v>
@@ -7802,7 +7529,7 @@
       </c>
       <c r="G17">
         <f t="shared" si="3"/>
-        <v>151031.56</v>
+        <v>128902.5</v>
       </c>
       <c r="H17" s="49" t="s">
         <v>95</v>
@@ -7822,7 +7549,7 @@
       <c r="M17" s="48"/>
       <c r="N17" s="48"/>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="str">
         <f t="shared" si="2"/>
         <v>XXXX (Ex: NBP2002)</v>
@@ -7847,7 +7574,7 @@
       </c>
       <c r="G18">
         <f t="shared" si="3"/>
-        <v>151031.56</v>
+        <v>128902.5</v>
       </c>
       <c r="H18" s="49" t="s">
         <v>95</v>
@@ -7864,7 +7591,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="str">
         <f t="shared" si="2"/>
         <v>XXXX (Ex: NBP2002)</v>
@@ -7889,7 +7616,7 @@
       </c>
       <c r="G19">
         <f t="shared" si="3"/>
-        <v>151031.56</v>
+        <v>128902.5</v>
       </c>
       <c r="H19" s="49" t="s">
         <v>95</v>
@@ -7906,85 +7633,85 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
       <c r="F20" s="14"/>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="22"/>
       <c r="D21" s="22"/>
       <c r="F21" s="14"/>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
       <c r="F23" s="14"/>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="22"/>
       <c r="D26" s="22"/>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
       <c r="F27" s="14"/>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
       <c r="F28" s="14"/>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="F29" s="14"/>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="22"/>
       <c r="D31" s="22"/>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="22"/>
@@ -8001,7 +7728,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AN44"/>
   <sheetViews>
@@ -8009,7 +7736,7 @@
       <selection activeCell="AA35" sqref="AA35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="7" width="8.85546875" style="1"/>
     <col min="8" max="8" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -8031,7 +7758,7 @@
     <col min="28" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" s="3" customFormat="1">
+    <row r="1" spans="1:40" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
@@ -8068,7 +7795,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:40" s="2" customFormat="1" ht="75">
+    <row r="2" spans="1:40" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -8172,7 +7899,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:40">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>45</v>
       </c>
@@ -8301,7 +8028,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>45</v>
       </c>
@@ -8430,7 +8157,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="5" spans="1:40">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>45</v>
       </c>
@@ -8559,7 +8286,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="6" spans="1:40">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>45</v>
       </c>
@@ -8688,7 +8415,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>45</v>
       </c>
@@ -8817,7 +8544,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="8" spans="1:40">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>45</v>
       </c>
@@ -8946,7 +8673,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="9" spans="1:40" s="32" customFormat="1">
+    <row r="9" spans="1:40" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
         <v>45</v>
       </c>
@@ -9075,7 +8802,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="10" spans="1:40">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>45</v>
       </c>
@@ -9204,7 +8931,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="11" spans="1:40">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>45</v>
       </c>
@@ -9333,7 +9060,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="12" spans="1:40">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>45</v>
       </c>
@@ -9462,7 +9189,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="13" spans="1:40">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>45</v>
       </c>
@@ -9591,7 +9318,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="14" spans="1:40">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>45</v>
       </c>
@@ -9720,7 +9447,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="15" spans="1:40">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>45</v>
       </c>
@@ -9849,7 +9576,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="16" spans="1:40">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>45</v>
       </c>
@@ -9978,7 +9705,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="17" spans="1:40">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A17" s="41" t="s">
         <v>45</v>
       </c>
@@ -10109,7 +9836,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="18" spans="1:40">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>45</v>
       </c>
@@ -10238,7 +9965,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="19" spans="1:40">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>45</v>
       </c>
@@ -10367,18 +10094,18 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="20" spans="1:40">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
       <c r="L20" s="20"/>
       <c r="M20" s="30"/>
       <c r="O20" s="30"/>
     </row>
-    <row r="21" spans="1:40">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
       <c r="D21" s="18"/>
       <c r="L21" s="20"/>
     </row>
-    <row r="22" spans="1:40">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
       <c r="D22" s="18"/>
       <c r="L22" s="20"/>
       <c r="M22" s="28"/>
@@ -10386,36 +10113,36 @@
       <c r="O22" s="28"/>
       <c r="R22" s="3"/>
     </row>
-    <row r="23" spans="1:40">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
       <c r="D23" s="18"/>
       <c r="L23" s="20"/>
       <c r="R23" s="3"/>
     </row>
-    <row r="24" spans="1:40">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
       <c r="D24" s="18"/>
       <c r="L24" s="20"/>
       <c r="R24" s="3"/>
     </row>
-    <row r="25" spans="1:40">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
       <c r="D25" s="18"/>
       <c r="L25" s="20"/>
       <c r="R25" s="3"/>
     </row>
-    <row r="26" spans="1:40">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
       <c r="D26" s="18"/>
       <c r="L26" s="20"/>
     </row>
-    <row r="27" spans="1:40">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
       <c r="D27" s="18"/>
       <c r="L27" s="20"/>
     </row>
-    <row r="28" spans="1:40">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
       <c r="D28" s="18"/>
       <c r="L28" s="28"/>
       <c r="M28" s="28"/>
       <c r="V28"/>
     </row>
-    <row r="29" spans="1:40">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
       <c r="D29" s="18"/>
       <c r="L29" s="20"/>
       <c r="R29" s="1">
@@ -10429,7 +10156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:40">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
       <c r="D30" s="18"/>
       <c r="L30" s="20"/>
       <c r="R30" s="1">
@@ -10447,7 +10174,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:40">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
       <c r="D31" s="18"/>
       <c r="L31" s="20"/>
       <c r="R31" s="1">
@@ -10465,7 +10192,7 @@
         <v>0.106033556646094</v>
       </c>
     </row>
-    <row r="32" spans="1:40">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
       <c r="D32" s="18"/>
       <c r="L32" s="20"/>
       <c r="R32" s="1">
@@ -10484,7 +10211,7 @@
         <v>8.4576498880189838E-2</v>
       </c>
     </row>
-    <row r="33" spans="4:22">
+    <row r="33" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D33" s="18"/>
       <c r="R33" s="1">
         <f t="shared" si="29"/>
@@ -10502,7 +10229,7 @@
         <v>-2.4700988419753349</v>
       </c>
     </row>
-    <row r="34" spans="4:22">
+    <row r="34" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D34" s="18"/>
       <c r="R34" s="1">
         <f t="shared" si="29"/>
@@ -10520,7 +10247,7 @@
         <v>79.680607805655967</v>
       </c>
     </row>
-    <row r="35" spans="4:22">
+    <row r="35" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D35" s="18"/>
       <c r="R35" s="1">
         <f t="shared" si="29"/>
@@ -10534,33 +10261,33 @@
         <v>133.80000000000001</v>
       </c>
     </row>
-    <row r="36" spans="4:22">
+    <row r="36" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D36" s="18"/>
     </row>
-    <row r="37" spans="4:22" ht="18.75">
+    <row r="37" spans="4:22" ht="18.75" x14ac:dyDescent="0.25">
       <c r="D37" s="18"/>
       <c r="R37" s="31"/>
     </row>
-    <row r="38" spans="4:22" ht="18.75">
+    <row r="38" spans="4:22" ht="18.75" x14ac:dyDescent="0.25">
       <c r="D38" s="18"/>
       <c r="R38" s="31"/>
     </row>
-    <row r="39" spans="4:22">
+    <row r="39" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D39" s="18"/>
     </row>
-    <row r="40" spans="4:22">
+    <row r="40" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D40" s="18"/>
     </row>
-    <row r="41" spans="4:22">
+    <row r="41" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D41" s="18"/>
     </row>
-    <row r="42" spans="4:22">
+    <row r="42" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D42" s="18"/>
     </row>
-    <row r="43" spans="4:22">
+    <row r="43" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D43" s="18"/>
     </row>
-    <row r="44" spans="4:22">
+    <row r="44" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D44" s="18"/>
     </row>
   </sheetData>
@@ -10577,9 +10304,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10806,27 +10536,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E25FD25F-4F7B-424B-B348-6FDF08E0D6BA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3389205F-2D79-473F-BF20-F5B4508DD860}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="a82fde31-7c4a-4ce9-9766-85cc00969e07"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="72ef6dce-e6e8-45af-a218-3a2d656dacd7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -10851,9 +10569,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3389205F-2D79-473F-BF20-F5B4508DD860}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E25FD25F-4F7B-424B-B348-6FDF08E0D6BA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="a82fde31-7c4a-4ce9-9766-85cc00969e07"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="72ef6dce-e6e8-45af-a218-3a2d656dacd7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>